<commit_message>
break out stock.yaml completed
</commit_message>
<xml_diff>
--- a/excel/1d/ph_pl_data_1d.xlsx
+++ b/excel/1d/ph_pl_data_1d.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G2404"/>
+  <dimension ref="A1:G2410"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -60549,6 +60549,156 @@
         <v>5600</v>
       </c>
     </row>
+    <row r="2405">
+      <c r="A2405" t="inlineStr">
+        <is>
+          <t>BATAINDIA.NS</t>
+        </is>
+      </c>
+      <c r="B2405" s="2" t="n">
+        <v>45356</v>
+      </c>
+      <c r="C2405" t="n">
+        <v>1473.849975585938</v>
+      </c>
+      <c r="D2405" t="n">
+        <v>1418.050048828125</v>
+      </c>
+      <c r="E2405" t="n">
+        <v>1448.75</v>
+      </c>
+      <c r="F2405" t="n">
+        <v>1</v>
+      </c>
+      <c r="G2405" t="n">
+        <v>1473.849975585938</v>
+      </c>
+    </row>
+    <row r="2406">
+      <c r="A2406" t="inlineStr">
+        <is>
+          <t>BATAINDIA.NS</t>
+        </is>
+      </c>
+      <c r="B2406" s="2" t="n">
+        <v>45394</v>
+      </c>
+      <c r="C2406" t="n">
+        <v>1404.400024414062</v>
+      </c>
+      <c r="D2406" t="n">
+        <v>1378.5</v>
+      </c>
+      <c r="E2406" t="n">
+        <v>1387.5</v>
+      </c>
+      <c r="F2406" t="n">
+        <v>1</v>
+      </c>
+      <c r="G2406" t="n">
+        <v>1404.400024414062</v>
+      </c>
+    </row>
+    <row r="2407">
+      <c r="A2407" t="inlineStr">
+        <is>
+          <t>BATAINDIA.NS</t>
+        </is>
+      </c>
+      <c r="B2407" s="2" t="n">
+        <v>45454</v>
+      </c>
+      <c r="C2407" t="n">
+        <v>1505.099975585938</v>
+      </c>
+      <c r="D2407" t="n">
+        <v>1470.599975585938</v>
+      </c>
+      <c r="E2407" t="n">
+        <v>1474.449951171875</v>
+      </c>
+      <c r="F2407" t="n">
+        <v>1</v>
+      </c>
+      <c r="G2407" t="n">
+        <v>1505.099975585938</v>
+      </c>
+    </row>
+    <row r="2408">
+      <c r="A2408" t="inlineStr">
+        <is>
+          <t>BATAINDIA.NS</t>
+        </is>
+      </c>
+      <c r="B2408" s="2" t="n">
+        <v>45401</v>
+      </c>
+      <c r="C2408" t="n">
+        <v>1341.699951171875</v>
+      </c>
+      <c r="D2408" t="n">
+        <v>1307.050048828125</v>
+      </c>
+      <c r="E2408" t="n">
+        <v>1320.400024414062</v>
+      </c>
+      <c r="F2408" t="n">
+        <v>2</v>
+      </c>
+      <c r="G2408" t="n">
+        <v>1307.050048828125</v>
+      </c>
+    </row>
+    <row r="2409">
+      <c r="A2409" t="inlineStr">
+        <is>
+          <t>BATAINDIA.NS</t>
+        </is>
+      </c>
+      <c r="B2409" s="2" t="n">
+        <v>45425</v>
+      </c>
+      <c r="C2409" t="n">
+        <v>1320.400024414062</v>
+      </c>
+      <c r="D2409" t="n">
+        <v>1294</v>
+      </c>
+      <c r="E2409" t="n">
+        <v>1317.199951171875</v>
+      </c>
+      <c r="F2409" t="n">
+        <v>2</v>
+      </c>
+      <c r="G2409" t="n">
+        <v>1294</v>
+      </c>
+    </row>
+    <row r="2410">
+      <c r="A2410" t="inlineStr">
+        <is>
+          <t>BATAINDIA.NS</t>
+        </is>
+      </c>
+      <c r="B2410" s="2" t="n">
+        <v>45447</v>
+      </c>
+      <c r="C2410" t="n">
+        <v>1372</v>
+      </c>
+      <c r="D2410" t="n">
+        <v>1269</v>
+      </c>
+      <c r="E2410" t="n">
+        <v>1337.199951171875</v>
+      </c>
+      <c r="F2410" t="n">
+        <v>2</v>
+      </c>
+      <c r="G2410" t="n">
+        <v>1269</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>